<commit_message>
Major update of slides
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_advanced_BA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6F1606-A057-B34E-92E8-34E1C1DD578C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8589479-7A74-434B-9A41-6D713D88BA4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -45,9 +45,6 @@
     <t>10:00-12:00</t>
   </si>
   <si>
-    <t>10:30-12:30</t>
-  </si>
-  <si>
     <t>Slides</t>
   </si>
   <si>
@@ -120,25 +117,61 @@
     <t>Labour · Labels</t>
   </si>
   <si>
-    <t>Wealth · Scales</t>
-  </si>
-  <si>
-    <t>Mobility · Waffles</t>
-  </si>
-  <si>
     <t>Growth · Geometries</t>
   </si>
   <si>
-    <t>Income · Themes</t>
-  </si>
-  <si>
     <t>04_growth</t>
   </si>
   <si>
     <t>05_inflation</t>
   </si>
   <si>
-    <t>Climate · Maps</t>
+    <t>Income · Scales</t>
+  </si>
+  <si>
+    <t>Wealth · Themes</t>
+  </si>
+  <si>
+    <t>Mobility · Maps</t>
+  </si>
+  <si>
+    <t>Climate · Facets</t>
+  </si>
+  <si>
+    <t>04_growth.R</t>
+  </si>
+  <si>
+    <t>05_inflation.R</t>
+  </si>
+  <si>
+    <t>02_data.RData</t>
+  </si>
+  <si>
+    <t>03_visualization.RData</t>
+  </si>
+  <si>
+    <t>04_growth.RData</t>
+  </si>
+  <si>
+    <t>05_inflation.RData</t>
+  </si>
+  <si>
+    <t>06_labour</t>
+  </si>
+  <si>
+    <t>06_labour.RData</t>
+  </si>
+  <si>
+    <t>06_labour.R</t>
+  </si>
+  <si>
+    <t>07_income</t>
+  </si>
+  <si>
+    <t>07_income.RData</t>
+  </si>
+  <si>
+    <t>07_income.Rmd</t>
   </si>
 </sst>
 </file>
@@ -148,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +191,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,10 +223,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -501,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15577C13-38EE-F34D-AF16-EA7AE3F3C88F}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,10 +553,11 @@
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
     <col min="5" max="6" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,19 +571,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44991</v>
       </c>
@@ -549,16 +594,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44998</v>
       </c>
@@ -566,25 +611,28 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45005</v>
       </c>
@@ -592,19 +640,22 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45012</v>
       </c>
@@ -612,19 +663,22 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45033</v>
       </c>
@@ -632,39 +686,51 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45040</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45054</v>
       </c>
@@ -672,13 +738,22 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45061</v>
       </c>
@@ -686,19 +761,19 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9">
+        <v>34</v>
+      </c>
+      <c r="H9">
         <v>3</v>
       </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45082</v>
       </c>
@@ -706,13 +781,13 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45089</v>
       </c>
@@ -720,19 +795,19 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11">
+        <v>36</v>
+      </c>
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45096</v>
       </c>
@@ -740,13 +815,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45103</v>
       </c>
@@ -754,10 +829,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add slides for climate lecture
</commit_message>
<xml_diff>
--- a/data/schedule/schedule.xlsx
+++ b/data/schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasschnetzer/Daten/Lehre/wipol_advanced_BA/data/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789A904F-AA88-C147-BB6B-9F9AB3712896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FB98FD-CC0D-2F45-9F32-DAA5CFCB9AE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F9BD3B2F-4F88-794D-B86A-6B2451FB96A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>09_mobility.RData</t>
+  </si>
+  <si>
+    <t>10_climate</t>
+  </si>
+  <si>
+    <t>10_climate.R</t>
+  </si>
+  <si>
+    <t>09_climate.RData</t>
   </si>
 </sst>
 </file>
@@ -563,7 +572,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,6 +845,15 @@
       <c r="D11" t="s">
         <v>36</v>
       </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
       <c r="H11">
         <v>4</v>
       </c>

</xml_diff>